<commit_message>
Test export of XLSX metadata
</commit_message>
<xml_diff>
--- a/tests/data/import/xlsx/sample_sentence/doc1.xlsx
+++ b/tests/data/import/xlsx/sample_sentence/doc1.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="meta" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">tok</t>
   </si>
@@ -59,6 +60,21 @@
   </si>
   <si>
     <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
   </si>
 </sst>
 </file>
@@ -73,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -132,8 +149,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -262,80 +287,89 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="2" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -350,4 +384,52 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2024</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add `skip_unchanged_files` config parameter to `xlsx` exporter.
</commit_message>
<xml_diff>
--- a/tests/data/import/xlsx/sample_sentence/doc1.xlsx
+++ b/tests/data/import/xlsx/sample_sentence/doc1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="meta" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">tok</t>
   </si>
@@ -32,6 +32,9 @@
     <t xml:space="preserve">Is</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">this</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
     <t xml:space="preserve">than</t>
   </si>
   <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
     <t xml:space="preserve">it</t>
   </si>
   <si>
@@ -75,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024</t>
   </si>
 </sst>
 </file>
@@ -158,7 +167,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,11 +296,11 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -305,69 +314,69 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -393,34 +402,34 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>14</v>
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>16</v>
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2024</v>
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>